<commit_message>
Test to verify error message for GB XXX locodes and removing errors that we dont show any more for GB Locode
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal1-Files/GDF1-arrival-errors.xlsx
+++ b/cypress/fixtures/Fal1-Files/GDF1-arrival-errors.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennikate/Desktop/nmswforms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW\nmsw-ui\cypress\fixtures\Fal1-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE062790-89AD-B049-AA2D-BB0E4747E0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BAFEC1-B518-47FD-A31F-173895E716C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12400" yWindow="500" windowWidth="23040" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAL 1" sheetId="1" r:id="rId1"/>
     <sheet name="ISO 3-letter country codes" sheetId="2" r:id="rId2"/>
     <sheet name="LOCODES" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2444,7 +2444,7 @@
     <t>GB ABD</t>
   </si>
   <si>
-    <t>GB XXX</t>
+    <t>GB DVR</t>
   </si>
 </sst>
 </file>
@@ -3367,6 +3367,21 @@
     <xf numFmtId="46" fontId="20" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3474,21 +3489,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4685,45 +4685,45 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31" style="25" customWidth="1"/>
     <col min="2" max="2" width="25" style="25" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" style="25" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="25" customWidth="1"/>
-    <col min="7" max="16" width="8.7109375" style="25" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="32.3828125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="27.3046875" style="25" customWidth="1"/>
+    <col min="5" max="5" width="31.84375" style="25" customWidth="1"/>
+    <col min="6" max="6" width="25.3828125" style="25" customWidth="1"/>
+    <col min="7" max="16" width="8.69140625" style="25" hidden="1" customWidth="1"/>
     <col min="17" max="16384" width="0" style="25" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-    </row>
-    <row r="2" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+    </row>
+    <row r="2" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>551</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="48"/>
-    </row>
-    <row r="3" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
+    </row>
+    <row r="3" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="149.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="149.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -4756,20 +4756,20 @@
       <c r="D4" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="E4" s="53"/>
-      <c r="F4" s="54"/>
-    </row>
-    <row r="5" spans="1:6" ht="270" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="58"/>
+      <c r="F4" s="59"/>
+    </row>
+    <row r="5" spans="1:6" ht="270" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="43" t="s">
         <v>553</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="80">
+      <c r="D5" s="44">
         <v>44978</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -4779,17 +4779,17 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="147.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="43" t="s">
         <v>552</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="81">
+      <c r="D6" s="45">
         <v>44979</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -4799,7 +4799,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="184.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="184.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -4809,17 +4809,17 @@
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="82" t="s">
+      <c r="D7" s="46" t="s">
         <v>556</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="83" t="s">
+      <c r="F7" s="47" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -4828,10 +4828,10 @@
         <v>17</v>
       </c>
       <c r="D8" s="39"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-    </row>
-    <row r="9" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+    </row>
+    <row r="9" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -4840,180 +4840,180 @@
         <v>19</v>
       </c>
       <c r="D9" s="34"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="49"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="55"/>
+      <c r="F9" s="54"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="33"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="49"/>
-    </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="60"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="54"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="34"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="49"/>
-    </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="62"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="54"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="35"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="49"/>
-    </row>
-    <row r="13" spans="1:6" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="62"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="54"/>
+    </row>
+    <row r="13" spans="1:6" ht="128.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="40" t="s">
         <v>554</v>
       </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="49"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="62"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="54"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="36"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="49"/>
-    </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="62"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="54"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="37"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="49"/>
-    </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="62"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="54"/>
+    </row>
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="33"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="49"/>
-    </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="51" t="s">
+      <c r="C16" s="62"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="54"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="49"/>
-    </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B17" s="57"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="54"/>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="26"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="49"/>
-    </row>
-    <row r="19" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+      <c r="C18" s="62"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="54"/>
+    </row>
+    <row r="19" spans="1:6" ht="33" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="26"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="49"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="62"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="54"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="26"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="49"/>
-    </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="54"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="49"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="62"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="54"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="26"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="49"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="62"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="54"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="26"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="49"/>
-    </row>
-    <row r="24" spans="1:6" ht="17.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="62"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="54"/>
+    </row>
+    <row r="24" spans="1:6" ht="17.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="49"/>
-    </row>
-    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="62"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="54"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="38"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="49"/>
-    </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="62"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="54"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="26"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="49"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5057,93 +5057,93 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" style="28" customWidth="1"/>
-    <col min="3" max="5" width="12.5703125" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="11.5703125" style="16"/>
+    <col min="1" max="1" width="12.53515625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="46.84375" style="28" customWidth="1"/>
+    <col min="3" max="5" width="12.53515625" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="11.53515625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="66"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="69"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="74"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="62"/>
-      <c r="E3" s="63"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="68"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="71"/>
-      <c r="E4" s="72"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="75"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="80"/>
       <c r="F5" s="19"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="76"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="78"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="83"/>
       <c r="F6" s="19"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
         <v>52</v>
       </c>
@@ -5154,7 +5154,7 @@
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
         <v>54</v>
       </c>
@@ -5165,7 +5165,7 @@
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="s">
         <v>56</v>
       </c>
@@ -5176,7 +5176,7 @@
       <c r="D9" s="14"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
         <v>58</v>
       </c>
@@ -5187,7 +5187,7 @@
       <c r="D10" s="14"/>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
         <v>60</v>
       </c>
@@ -5198,7 +5198,7 @@
       <c r="D11" s="14"/>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="27" t="s">
         <v>62</v>
       </c>
@@ -5209,7 +5209,7 @@
       <c r="D12" s="14"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="27" t="s">
         <v>64</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
         <v>66</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
         <v>68</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="27" t="s">
         <v>70</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="27" t="s">
         <v>72</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="27" t="s">
         <v>74</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="27" t="s">
         <v>76</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="27" t="s">
         <v>78</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="27" t="s">
         <v>80</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="27" t="s">
         <v>82</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="27" t="s">
         <v>84</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="27" t="s">
         <v>86</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="27" t="s">
         <v>88</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="27" t="s">
         <v>90</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="27" t="s">
         <v>92</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="27" t="s">
         <v>94</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="27" t="s">
         <v>96</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="27" t="s">
         <v>98</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="27" t="s">
         <v>100</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="27" t="s">
         <v>102</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="27" t="s">
         <v>104</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="27" t="s">
         <v>106</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="27" t="s">
         <v>108</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="27" t="s">
         <v>110</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="27" t="s">
         <v>112</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="27" t="s">
         <v>114</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="27" t="s">
         <v>116</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="27" t="s">
         <v>118</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="27" t="s">
         <v>120</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="27" t="s">
         <v>122</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="27" t="s">
         <v>124</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="27" t="s">
         <v>126</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="27" t="s">
         <v>128</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="27" t="s">
         <v>130</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="27" t="s">
         <v>132</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="27" t="s">
         <v>134</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="27" t="s">
         <v>136</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="27" t="s">
         <v>138</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="27" t="s">
         <v>140</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="27" t="s">
         <v>142</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="27" t="s">
         <v>144</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="27" t="s">
         <v>146</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="27" t="s">
         <v>148</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="27" t="s">
         <v>150</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="27" t="s">
         <v>152</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="27" t="s">
         <v>154</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="27" t="s">
         <v>156</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="27" t="s">
         <v>158</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="27" t="s">
         <v>160</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="27" t="s">
         <v>162</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="27" t="s">
         <v>164</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="27" t="s">
         <v>166</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="27" t="s">
         <v>168</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="27" t="s">
         <v>170</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="27" t="s">
         <v>172</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="27" t="s">
         <v>174</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="27" t="s">
         <v>176</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="27" t="s">
         <v>178</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="27" t="s">
         <v>180</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="27" t="s">
         <v>182</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="27" t="s">
         <v>184</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="27" t="s">
         <v>186</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="27" t="s">
         <v>188</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="27" t="s">
         <v>190</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="27" t="s">
         <v>192</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="27" t="s">
         <v>194</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="27" t="s">
         <v>196</v>
       </c>
@@ -5745,7 +5745,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="27" t="s">
         <v>198</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="27" t="s">
         <v>200</v>
       </c>
@@ -5761,7 +5761,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="27" t="s">
         <v>202</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="27" t="s">
         <v>204</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="27" t="s">
         <v>206</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="27" t="s">
         <v>208</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="27" t="s">
         <v>210</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="27" t="s">
         <v>212</v>
       </c>
@@ -5809,7 +5809,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="27" t="s">
         <v>214</v>
       </c>
@@ -5817,7 +5817,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="27" t="s">
         <v>216</v>
       </c>
@@ -5825,7 +5825,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="27" t="s">
         <v>218</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="27" t="s">
         <v>220</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="27" t="s">
         <v>222</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="27" t="s">
         <v>224</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="27" t="s">
         <v>226</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="27" t="s">
         <v>228</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="27" t="s">
         <v>230</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="27" t="s">
         <v>232</v>
       </c>
@@ -5889,7 +5889,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="27" t="s">
         <v>234</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="27" t="s">
         <v>236</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="27" t="s">
         <v>238</v>
       </c>
@@ -5913,7 +5913,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="27" t="s">
         <v>240</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="27" t="s">
         <v>242</v>
       </c>
@@ -5929,7 +5929,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="27" t="s">
         <v>244</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="27" t="s">
         <v>246</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="27" t="s">
         <v>248</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="27" t="s">
         <v>250</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="27" t="s">
         <v>252</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="27" t="s">
         <v>254</v>
       </c>
@@ -5977,7 +5977,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="27" t="s">
         <v>256</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="27" t="s">
         <v>258</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="27" t="s">
         <v>260</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="27" t="s">
         <v>262</v>
       </c>
@@ -6009,7 +6009,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="27" t="s">
         <v>264</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="27" t="s">
         <v>266</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="27" t="s">
         <v>268</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="27" t="s">
         <v>270</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="27" t="s">
         <v>272</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="27" t="s">
         <v>274</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="27" t="s">
         <v>276</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="27" t="s">
         <v>278</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="27" t="s">
         <v>280</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="27" t="s">
         <v>282</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="27" t="s">
         <v>284</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="27" t="s">
         <v>286</v>
       </c>
@@ -6105,7 +6105,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="27" t="s">
         <v>288</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="27" t="s">
         <v>290</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="27" t="s">
         <v>292</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="27" t="s">
         <v>294</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="27" t="s">
         <v>296</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="27" t="s">
         <v>298</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="27" t="s">
         <v>300</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="27" t="s">
         <v>302</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="27" t="s">
         <v>304</v>
       </c>
@@ -6177,7 +6177,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="27" t="s">
         <v>306</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="27" t="s">
         <v>308</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="27" t="s">
         <v>310</v>
       </c>
@@ -6201,7 +6201,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="27" t="s">
         <v>312</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="27" t="s">
         <v>314</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="27" t="s">
         <v>316</v>
       </c>
@@ -6225,7 +6225,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="27" t="s">
         <v>318</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="27" t="s">
         <v>320</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="27" t="s">
         <v>322</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="27" t="s">
         <v>324</v>
       </c>
@@ -6257,7 +6257,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="27" t="s">
         <v>326</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="27" t="s">
         <v>328</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="27" t="s">
         <v>330</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="27" t="s">
         <v>332</v>
       </c>
@@ -6289,7 +6289,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="27" t="s">
         <v>334</v>
       </c>
@@ -6297,7 +6297,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="27" t="s">
         <v>336</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="27" t="s">
         <v>338</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="27" t="s">
         <v>340</v>
       </c>
@@ -6321,7 +6321,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="27" t="s">
         <v>342</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="27" t="s">
         <v>344</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="27" t="s">
         <v>346</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="27" t="s">
         <v>348</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="27" t="s">
         <v>350</v>
       </c>
@@ -6361,7 +6361,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="27" t="s">
         <v>352</v>
       </c>
@@ -6369,7 +6369,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="27" t="s">
         <v>354</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="27" t="s">
         <v>356</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="27" t="s">
         <v>358</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="27" t="s">
         <v>360</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="27" t="s">
         <v>362</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="27" t="s">
         <v>364</v>
       </c>
@@ -6417,7 +6417,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="27" t="s">
         <v>366</v>
       </c>
@@ -6425,7 +6425,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="27" t="s">
         <v>368</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="27" t="s">
         <v>370</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="27" t="s">
         <v>372</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="27" t="s">
         <v>374</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="27" t="s">
         <v>376</v>
       </c>
@@ -6465,7 +6465,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="27" t="s">
         <v>378</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="27" t="s">
         <v>380</v>
       </c>
@@ -6481,7 +6481,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="27" t="s">
         <v>382</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="27" t="s">
         <v>384</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="27" t="s">
         <v>386</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="27" t="s">
         <v>388</v>
       </c>
@@ -6513,7 +6513,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="27" t="s">
         <v>390</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="27" t="s">
         <v>392</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="27" t="s">
         <v>394</v>
       </c>
@@ -6537,7 +6537,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="27" t="s">
         <v>396</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="27" t="s">
         <v>398</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="27" t="s">
         <v>400</v>
       </c>
@@ -6561,7 +6561,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="27" t="s">
         <v>402</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="27" t="s">
         <v>404</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="27" t="s">
         <v>406</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="27" t="s">
         <v>408</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="27" t="s">
         <v>410</v>
       </c>
@@ -6601,7 +6601,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="27" t="s">
         <v>412</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="27" t="s">
         <v>414</v>
       </c>
@@ -6617,7 +6617,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="27" t="s">
         <v>416</v>
       </c>
@@ -6625,7 +6625,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" s="27" t="s">
         <v>418</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="27" t="s">
         <v>420</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="27" t="s">
         <v>422</v>
       </c>
@@ -6649,7 +6649,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="27" t="s">
         <v>424</v>
       </c>
@@ -6657,7 +6657,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="27" t="s">
         <v>426</v>
       </c>
@@ -6665,7 +6665,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="27" t="s">
         <v>428</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" s="27" t="s">
         <v>430</v>
       </c>
@@ -6681,7 +6681,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" s="27" t="s">
         <v>432</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="27" t="s">
         <v>434</v>
       </c>
@@ -6697,7 +6697,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="27" t="s">
         <v>436</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" s="27" t="s">
         <v>438</v>
       </c>
@@ -6713,7 +6713,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="27" t="s">
         <v>440</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="27" t="s">
         <v>442</v>
       </c>
@@ -6729,7 +6729,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="27" t="s">
         <v>444</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" s="27" t="s">
         <v>446</v>
       </c>
@@ -6745,7 +6745,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="27" t="s">
         <v>448</v>
       </c>
@@ -6753,7 +6753,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="27" t="s">
         <v>450</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" s="27" t="s">
         <v>452</v>
       </c>
@@ -6769,7 +6769,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" s="27" t="s">
         <v>454</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" s="27" t="s">
         <v>456</v>
       </c>
@@ -6785,7 +6785,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="27" t="s">
         <v>458</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="27" t="s">
         <v>460</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="27" t="s">
         <v>462</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" s="27" t="s">
         <v>464</v>
       </c>
@@ -6817,7 +6817,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" s="27" t="s">
         <v>466</v>
       </c>
@@ -6825,7 +6825,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="27" t="s">
         <v>468</v>
       </c>
@@ -6833,7 +6833,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="27" t="s">
         <v>470</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="27" t="s">
         <v>472</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="27" t="s">
         <v>474</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" s="27" t="s">
         <v>476</v>
       </c>
@@ -6865,7 +6865,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="27" t="s">
         <v>478</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" s="27" t="s">
         <v>480</v>
       </c>
@@ -6881,7 +6881,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="27" t="s">
         <v>482</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" s="27" t="s">
         <v>484</v>
       </c>
@@ -6897,7 +6897,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A224" s="27" t="s">
         <v>486</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A225" s="27" t="s">
         <v>488</v>
       </c>
@@ -6913,7 +6913,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A226" s="27" t="s">
         <v>490</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A227" s="27" t="s">
         <v>492</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A228" s="27" t="s">
         <v>494</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A229" s="27" t="s">
         <v>496</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A230" s="27" t="s">
         <v>498</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A231" s="27" t="s">
         <v>500</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A232" s="27" t="s">
         <v>502</v>
       </c>
@@ -6969,7 +6969,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A233" s="27" t="s">
         <v>504</v>
       </c>
@@ -6977,7 +6977,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A234" s="27" t="s">
         <v>506</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A235" s="27" t="s">
         <v>508</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A236" s="27" t="s">
         <v>510</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A237" s="27" t="s">
         <v>512</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A238" s="27" t="s">
         <v>514</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A239" s="27" t="s">
         <v>516</v>
       </c>
@@ -7025,7 +7025,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A240" s="27" t="s">
         <v>518</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A241" s="27" t="s">
         <v>520</v>
       </c>
@@ -7041,7 +7041,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A242" s="27" t="s">
         <v>522</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A243" s="27" t="s">
         <v>524</v>
       </c>
@@ -7057,7 +7057,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A244" s="27" t="s">
         <v>526</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A245" s="27" t="s">
         <v>528</v>
       </c>
@@ -7073,7 +7073,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A246" s="27" t="s">
         <v>530</v>
       </c>
@@ -7081,7 +7081,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A247" s="27" t="s">
         <v>532</v>
       </c>
@@ -7089,7 +7089,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A248" s="27" t="s">
         <v>534</v>
       </c>
@@ -7097,7 +7097,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A249" s="27" t="s">
         <v>536</v>
       </c>
@@ -7105,7 +7105,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A250" s="27" t="s">
         <v>538</v>
       </c>
@@ -7113,7 +7113,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="251" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A251" s="27" t="s">
         <v>540</v>
       </c>
@@ -7121,7 +7121,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="252" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A252" s="27" t="s">
         <v>542</v>
       </c>
@@ -7129,7 +7129,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A253" s="27" t="s">
         <v>544</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A254" s="27" t="s">
         <v>546</v>
       </c>
@@ -7170,27 +7170,27 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="47.3828125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.69140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.69140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="23"/>
     </row>
-    <row r="4" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
         <v>550</v>
       </c>
@@ -7208,6 +7208,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D364DC965387FD4EAF4833DDCF640F91" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c7401bc8bddc44f3d87e6545050f3282">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18390984-f7d9-4502-80ba-82ec344db5fb" xmlns:ns3="629dd2dc-abea-47e8-ba88-82202e3ee8ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3cb6a02f8baa81433631181c409fee" ns2:_="" ns3:_="">
     <xsd:import namespace="18390984-f7d9-4502-80ba-82ec344db5fb"/>
@@ -7444,27 +7464,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
+    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A6CC910-0FFF-41DD-A80E-A1312D067115}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7481,23 +7500,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
-    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>